<commit_message>
Move to Guzzle6 so I can use promises Continue work on account importer
</commit_message>
<xml_diff>
--- a/templates/Services.xlsx
+++ b/templates/Services.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -35,7 +35,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">The ID of the account. Must already exist in Sonar.</t>
+          <t xml:space="preserve">A descriptive name for the service.</t>
         </r>
       </text>
     </comment>
@@ -48,7 +48,163 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">This should be entered as a number, no currency symbol. Enter a negative number if the customer is owed services (e.g. they overpaid) and a positive number if they have an unpaid balance. </t>
+          <t xml:space="preserve">One of ‘one time’, ‘recurring’, ‘expiring’, ‘adjustment’, ‘overage’</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">One of ‘credit’, ‘debit’</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">The amount to be debited from, or credited to the account when this service is used.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">If this service is an expiring service, enter the number of times the service runs here. This is required if the service is of type ‘expiring’</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Enter the IDs of taxes to be associated with this service here, separated by commas. These taxes must already exist in Sonar, and you must use the tax IDs from within Sonar.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Set this to 1 if this is a data service, 0 if it is not. Only recurring services can be data services.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Download speed in kilobits per second. This is required if data service is ‘1’</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">The upload speed in kilobits per second. This is required if data service is ‘1’</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">The technology code for the service. Only required if this is a data service. This is mostly used for generating the FCC Form 477 report, and the integers correspond to the following types. 0 = Other, 10 = Asymmetric xDSL, 20 = Symmetric xDSL, 30 = Copper Wireline, 40 = Cable Modem, 50 = Fiber, 60 = Satellite, 70 = Terrestrial Fixed Wireless, 90 = Electric Power Line.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">The ID of a usage based billing policy to apply to this service. Only applicable to data services, and not required.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">If the type of service is ‘Overage’, this is number of gigabytes given by the overage service. Required for overage services.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">If you want to associate a general ledger code with this service, enter an existing general ledger code ID here. This must already been created in Sonar.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">The amount of the service to exempt from taxation.</t>
         </r>
       </text>
     </comment>
@@ -57,12 +213,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t xml:space="preserve">Account ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prior Balance</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Times to Run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taxes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Download (Kilobits per second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upload (Kilobits per second)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technology Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usage Based Billing Policy ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit Quantity in Gigabytes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General Ledger Code ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tax Exemption Amount</t>
   </si>
 </sst>
 </file>
@@ -108,7 +300,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -119,6 +311,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00CCFF"/>
+        <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -156,12 +354,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -293,7 +495,87 @@
               </a:uFill>
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
-            <a:t>This template is used to update balances on existing customer accounts. This can be used if you want to import your accounts first, validate them, and then later import balances before you bill.</a:t>
+            <a:t>This template is used to import services into Sonar. Please bear in mind that this import document is necessarily complex, and requires an understanding of some of the different fields for services within Sonar.</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>If in doubt, it is often easier to create services by hand inside Sonar to ensure proper application of taxes, service speeds, voice service definitions, etc.</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>Blue columns are not required, grey columns are required.</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:solidFill>
@@ -321,7 +603,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="P14" activeCellId="0" sqref="P14"/>
     </sheetView>
   </sheetViews>
@@ -347,14 +629,27 @@
   </sheetPr>
   <dimension ref="1:1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X9" activeCellId="0" sqref="X9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.515306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.0459183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8214285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.1530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="35.4285714285714"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.1836734693878"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.7602040816327"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="33.3163265306122"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.5102040816327"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="27.25"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="26.6836734693878"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.2448979591837"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -363,6 +658,42 @@
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="ALL1" s="0"/>
       <c r="ALM1" s="0"/>

</xml_diff>

<commit_message>
Add an option to set the ID when importing services
</commit_message>
<xml_diff>
--- a/templates/Services.xlsx
+++ b/templates/Services.xlsx
@@ -195,12 +195,25 @@
         </r>
       </text>
     </comment>
+    <comment ref="N1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">If you need this service to have a specific ID, enter it here. This is mostly useful when importing from other systems. The ID must be unique, and must be an integer of 1 or greater.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -239,6 +252,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tax Exemption Amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service ID</t>
   </si>
 </sst>
 </file>
@@ -434,9 +450,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>104760</xdr:colOff>
+      <xdr:colOff>104400</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>38520</xdr:rowOff>
+      <xdr:rowOff>38160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -446,7 +462,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="108000" y="1800"/>
-          <a:ext cx="6597360" cy="8327880"/>
+          <a:ext cx="6492240" cy="8327520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -593,7 +609,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -617,26 +633,26 @@
   <dimension ref="1:1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="34.9642857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="31.7244897959184"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="32.8010204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="26.3214285714286"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="34.5561224489796"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="32.3979591836735"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -678,6 +694,9 @@
       </c>
       <c r="M1" s="2" t="s">
         <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="ALK1" s="0"/>
       <c r="ALL1" s="0"/>

</xml_diff>

<commit_message>
Allow the import of one time/adjustment services
</commit_message>
<xml_diff>
--- a/templates/Services.xlsx
+++ b/templates/Services.xlsx
@@ -48,7 +48,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">One of ‘one time’, ‘recurring’, ‘expiring’</t>
+          <t xml:space="preserve">One of ‘one time’, ‘recurring’, ‘expiring’, ‘one time’, or ‘adjustment’</t>
         </r>
       </text>
     </comment>
@@ -450,9 +450,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>104400</xdr:colOff>
+      <xdr:colOff>104040</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:rowOff>37800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -462,7 +462,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="108000" y="1800"/>
-          <a:ext cx="6492240" cy="8327520"/>
+          <a:ext cx="6491880" cy="8327160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -603,20 +603,20 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="P14" activeCellId="0" sqref="P14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -630,29 +630,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:1"/>
+  <dimension ref="A1:AMJ1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="34.5561224489796"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="34.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="31.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="32.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="26.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="25.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="15.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -728,7 +728,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>